<commit_message>
Tried making new channel maps
New channel maps for 1x32 flex design from Pavlo's CAD file. They don't work for this batch of devices (Rh7 and beyond). It seems like the AutoCAD file provided doesn't match the device being implanted
</commit_message>
<xml_diff>
--- a/Channel_Maps/excels/chan_map_1x32_128ch_flex.xlsx
+++ b/Channel_Maps/excels/chan_map_1x32_128ch_flex.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26712"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\Research Work at RICE\Research\Channel_Map\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D7C6A4E-8D43-41D9-980D-2AA54F8AFE6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{444CBCC9-D6C8-46D0-B2CD-F72433CC2FCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-17388" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{A98CB213-382E-42E1-BAA3-E8593D5458F5}"/>
+    <workbookView xWindow="-108" yWindow="-17388" windowWidth="30936" windowHeight="16776" xr2:uid="{A98CB213-382E-42E1-BAA3-E8593D5458F5}"/>
   </bookViews>
   <sheets>
     <sheet name="Flex PCB" sheetId="1" r:id="rId1"/>
     <sheet name="PCB_Intan" sheetId="2" r:id="rId2"/>
     <sheet name="Device_Intan" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,6 +29,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -36,444 +38,453 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="151">
+  <si>
+    <t>1,31</t>
+  </si>
+  <si>
+    <t>1,13</t>
+  </si>
+  <si>
+    <t>2,27</t>
+  </si>
+  <si>
+    <t>2,9</t>
+  </si>
+  <si>
+    <t>3,23</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>4,19</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>1,32</t>
+  </si>
+  <si>
+    <t>1,12</t>
+  </si>
+  <si>
+    <t>2,26</t>
+  </si>
+  <si>
+    <t>2,8</t>
+  </si>
+  <si>
+    <t>3,22</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>4,18</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>1,30</t>
+  </si>
+  <si>
+    <t>1,11</t>
+  </si>
+  <si>
+    <t>2,25</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>3,21</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,17</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>1,29</t>
+  </si>
+  <si>
+    <t>1,10</t>
+  </si>
+  <si>
+    <t>2,24</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>3,20</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>4,20</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>1,28</t>
+  </si>
+  <si>
+    <t>1,9</t>
+  </si>
+  <si>
+    <t>2,23</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>3,19</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>4,21</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>1,27</t>
+  </si>
+  <si>
+    <t>1,8</t>
+  </si>
+  <si>
+    <t>2,22</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>3,18</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>4,22</t>
+  </si>
+  <si>
+    <t>4,6</t>
+  </si>
+  <si>
+    <t>1,26</t>
+  </si>
+  <si>
+    <t>1,7</t>
+  </si>
+  <si>
+    <t>2,21</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>3,17</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>4,23</t>
+  </si>
+  <si>
+    <t>4,7</t>
+  </si>
+  <si>
+    <t>1,25</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>2,20</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,24</t>
+  </si>
+  <si>
+    <t>3,8</t>
+  </si>
+  <si>
+    <t>4,24</t>
+  </si>
+  <si>
+    <t>4,8</t>
+  </si>
+  <si>
+    <t>1,24</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>2,19</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>3,25</t>
+  </si>
+  <si>
+    <t>3,9</t>
+  </si>
+  <si>
+    <t>4,25</t>
+  </si>
+  <si>
+    <t>4,9</t>
+  </si>
+  <si>
+    <t>1,23</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>2,18</t>
+  </si>
+  <si>
+    <t>2,10</t>
+  </si>
+  <si>
+    <t>3,26</t>
+  </si>
+  <si>
+    <t>3,10</t>
+  </si>
+  <si>
+    <t>4,26</t>
+  </si>
+  <si>
+    <t>4,10</t>
+  </si>
+  <si>
+    <t>1,22</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>2,17</t>
+  </si>
+  <si>
+    <t>2,11</t>
+  </si>
+  <si>
+    <t>3,27</t>
+  </si>
+  <si>
+    <t>3,11</t>
+  </si>
+  <si>
+    <t>4,27</t>
+  </si>
+  <si>
+    <t>4,11</t>
+  </si>
+  <si>
+    <t>1,21</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>2,28</t>
+  </si>
+  <si>
+    <t>2,12</t>
+  </si>
+  <si>
+    <t>3,28</t>
+  </si>
+  <si>
+    <t>3,12</t>
+  </si>
+  <si>
+    <t>4,28</t>
+  </si>
+  <si>
+    <t>4,12</t>
+  </si>
+  <si>
+    <t>1,20</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>2,29</t>
+  </si>
+  <si>
+    <t>2,13</t>
+  </si>
+  <si>
+    <t>3,29</t>
+  </si>
+  <si>
+    <t>3,13</t>
+  </si>
+  <si>
+    <t>4,29</t>
+  </si>
+  <si>
+    <t>4,13</t>
+  </si>
+  <si>
+    <t>1,19</t>
+  </si>
+  <si>
+    <t>1,14</t>
+  </si>
+  <si>
+    <t>2,30</t>
+  </si>
+  <si>
+    <t>2,14</t>
+  </si>
+  <si>
+    <t>3,30</t>
+  </si>
+  <si>
+    <t>3,14</t>
+  </si>
+  <si>
+    <t>4,30</t>
+  </si>
+  <si>
+    <t>4,14</t>
+  </si>
+  <si>
+    <t>1,18</t>
+  </si>
+  <si>
+    <t>1,15</t>
+  </si>
+  <si>
+    <t>2,32</t>
+  </si>
+  <si>
+    <t>2,15</t>
+  </si>
+  <si>
+    <t>3,32</t>
+  </si>
+  <si>
+    <t>3,15</t>
+  </si>
+  <si>
+    <t>4,32</t>
+  </si>
+  <si>
+    <t>4,15</t>
+  </si>
+  <si>
+    <t>1,17</t>
+  </si>
+  <si>
+    <t>1,16</t>
+  </si>
+  <si>
+    <t>2,31</t>
+  </si>
+  <si>
+    <t>2,16</t>
+  </si>
+  <si>
+    <t>3,31</t>
+  </si>
+  <si>
+    <t>3,16</t>
+  </si>
+  <si>
+    <t>4,31</t>
+  </si>
+  <si>
+    <t>4,16</t>
+  </si>
+  <si>
+    <t>NAN</t>
+  </si>
+  <si>
+    <t>1x32 flex NEW PAVLO</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
   <si>
     <t>FLEX PCB BACKEND U3</t>
   </si>
   <si>
-    <t>NAN</t>
-  </si>
-  <si>
     <t>FLEX PCB BACKEND U4</t>
   </si>
   <si>
-    <t>U2</t>
-  </si>
-  <si>
-    <t>U1</t>
+    <t>32 means shallow</t>
+  </si>
+  <si>
+    <t>1 means deep</t>
+  </si>
+  <si>
+    <t>Orientation shown</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>This is the flex PCB mapping</t>
+  </si>
+  <si>
+    <t>Connecting the device to the flex PCB yields this</t>
+  </si>
+  <si>
+    <t>Showing metal pins side (metal pins visible on this side)</t>
+  </si>
+  <si>
+    <t>MAP THIS TO "KLMNO" next sheet</t>
+  </si>
+  <si>
+    <t>Flip horizontally!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b/c we actually connect </t>
+  </si>
+  <si>
+    <t xml:space="preserve">U4 (flex pcb layout) to </t>
+  </si>
+  <si>
+    <t>U1 (rigid pcb adapter)</t>
   </si>
   <si>
     <t>na</t>
   </si>
   <si>
-    <t>U4</t>
-  </si>
-  <si>
-    <t>U3</t>
-  </si>
-  <si>
     <t>Letters here</t>
-  </si>
-  <si>
-    <t>4,1</t>
-  </si>
-  <si>
-    <t>1,31</t>
-  </si>
-  <si>
-    <t>1,32</t>
-  </si>
-  <si>
-    <t>1,30</t>
-  </si>
-  <si>
-    <t>1,13</t>
-  </si>
-  <si>
-    <t>2,27</t>
-  </si>
-  <si>
-    <t>2,9</t>
-  </si>
-  <si>
-    <t>3,23</t>
-  </si>
-  <si>
-    <t>3,5</t>
-  </si>
-  <si>
-    <t>4,19</t>
-  </si>
-  <si>
-    <t>1,12</t>
-  </si>
-  <si>
-    <t>2,26</t>
-  </si>
-  <si>
-    <t>2,8</t>
-  </si>
-  <si>
-    <t>3,22</t>
-  </si>
-  <si>
-    <t>3,4</t>
-  </si>
-  <si>
-    <t>4,18</t>
-  </si>
-  <si>
-    <t>4,2</t>
-  </si>
-  <si>
-    <t>1,11</t>
-  </si>
-  <si>
-    <t>2,25</t>
-  </si>
-  <si>
-    <t>2,7</t>
-  </si>
-  <si>
-    <t>3,21</t>
-  </si>
-  <si>
-    <t>3,3</t>
-  </si>
-  <si>
-    <t>4,17</t>
-  </si>
-  <si>
-    <t>4,3</t>
-  </si>
-  <si>
-    <t>1,29</t>
-  </si>
-  <si>
-    <t>1,10</t>
-  </si>
-  <si>
-    <t>2,24</t>
-  </si>
-  <si>
-    <t>2,6</t>
-  </si>
-  <si>
-    <t>3,20</t>
-  </si>
-  <si>
-    <t>3,2</t>
-  </si>
-  <si>
-    <t>4,20</t>
-  </si>
-  <si>
-    <t>4,4</t>
-  </si>
-  <si>
-    <t>1,28</t>
-  </si>
-  <si>
-    <t>1,9</t>
-  </si>
-  <si>
-    <t>2,23</t>
-  </si>
-  <si>
-    <t>2,5</t>
-  </si>
-  <si>
-    <t>3,19</t>
-  </si>
-  <si>
-    <t>3,1</t>
-  </si>
-  <si>
-    <t>4,21</t>
-  </si>
-  <si>
-    <t>4,5</t>
-  </si>
-  <si>
-    <t>1,27</t>
-  </si>
-  <si>
-    <t>1,8</t>
-  </si>
-  <si>
-    <t>2,22</t>
-  </si>
-  <si>
-    <t>2,4</t>
-  </si>
-  <si>
-    <t>3,18</t>
-  </si>
-  <si>
-    <t>3,6</t>
-  </si>
-  <si>
-    <t>4,22</t>
-  </si>
-  <si>
-    <t>4,6</t>
-  </si>
-  <si>
-    <t>1,26</t>
-  </si>
-  <si>
-    <t>1,7</t>
-  </si>
-  <si>
-    <t>2,21</t>
-  </si>
-  <si>
-    <t>2,3</t>
-  </si>
-  <si>
-    <t>3,17</t>
-  </si>
-  <si>
-    <t>3,7</t>
-  </si>
-  <si>
-    <t>4,23</t>
-  </si>
-  <si>
-    <t>4,7</t>
-  </si>
-  <si>
-    <t>1,25</t>
-  </si>
-  <si>
-    <t>1,6</t>
-  </si>
-  <si>
-    <t>2,20</t>
-  </si>
-  <si>
-    <t>2,2</t>
-  </si>
-  <si>
-    <t>3,24</t>
-  </si>
-  <si>
-    <t>3,8</t>
-  </si>
-  <si>
-    <t>4,24</t>
-  </si>
-  <si>
-    <t>4,8</t>
-  </si>
-  <si>
-    <t>1,24</t>
-  </si>
-  <si>
-    <t>1,5</t>
-  </si>
-  <si>
-    <t>2,19</t>
-  </si>
-  <si>
-    <t>2,1</t>
-  </si>
-  <si>
-    <t>3,25</t>
-  </si>
-  <si>
-    <t>3,9</t>
-  </si>
-  <si>
-    <t>4,25</t>
-  </si>
-  <si>
-    <t>4,9</t>
-  </si>
-  <si>
-    <t>1,23</t>
-  </si>
-  <si>
-    <t>1,4</t>
-  </si>
-  <si>
-    <t>2,18</t>
-  </si>
-  <si>
-    <t>2,10</t>
-  </si>
-  <si>
-    <t>3,26</t>
-  </si>
-  <si>
-    <t>3,10</t>
-  </si>
-  <si>
-    <t>4,26</t>
-  </si>
-  <si>
-    <t>4,10</t>
-  </si>
-  <si>
-    <t>1,22</t>
-  </si>
-  <si>
-    <t>1,3</t>
-  </si>
-  <si>
-    <t>2,17</t>
-  </si>
-  <si>
-    <t>2,11</t>
-  </si>
-  <si>
-    <t>3,27</t>
-  </si>
-  <si>
-    <t>3,11</t>
-  </si>
-  <si>
-    <t>4,27</t>
-  </si>
-  <si>
-    <t>4,11</t>
-  </si>
-  <si>
-    <t>1,21</t>
-  </si>
-  <si>
-    <t>1,2</t>
-  </si>
-  <si>
-    <t>2,28</t>
-  </si>
-  <si>
-    <t>2,12</t>
-  </si>
-  <si>
-    <t>3,28</t>
-  </si>
-  <si>
-    <t>3,12</t>
-  </si>
-  <si>
-    <t>4,28</t>
-  </si>
-  <si>
-    <t>4,12</t>
-  </si>
-  <si>
-    <t>1,20</t>
-  </si>
-  <si>
-    <t>1,1</t>
-  </si>
-  <si>
-    <t>2,29</t>
-  </si>
-  <si>
-    <t>2,13</t>
-  </si>
-  <si>
-    <t>3,29</t>
-  </si>
-  <si>
-    <t>3,13</t>
-  </si>
-  <si>
-    <t>4,29</t>
-  </si>
-  <si>
-    <t>4,13</t>
-  </si>
-  <si>
-    <t>1,19</t>
-  </si>
-  <si>
-    <t>1,14</t>
-  </si>
-  <si>
-    <t>2,30</t>
-  </si>
-  <si>
-    <t>2,14</t>
-  </si>
-  <si>
-    <t>3,30</t>
-  </si>
-  <si>
-    <t>3,14</t>
-  </si>
-  <si>
-    <t>4,30</t>
-  </si>
-  <si>
-    <t>4,14</t>
-  </si>
-  <si>
-    <t>1,18</t>
-  </si>
-  <si>
-    <t>1,15</t>
-  </si>
-  <si>
-    <t>2,32</t>
-  </si>
-  <si>
-    <t>2,15</t>
-  </si>
-  <si>
-    <t>3,32</t>
-  </si>
-  <si>
-    <t>3,15</t>
-  </si>
-  <si>
-    <t>4,32</t>
-  </si>
-  <si>
-    <t>4,15</t>
-  </si>
-  <si>
-    <t>1,17</t>
-  </si>
-  <si>
-    <t>1,16</t>
-  </si>
-  <si>
-    <t>2,31</t>
-  </si>
-  <si>
-    <t>2,16</t>
-  </si>
-  <si>
-    <t>3,31</t>
-  </si>
-  <si>
-    <t>3,16</t>
-  </si>
-  <si>
-    <t>4,31</t>
-  </si>
-  <si>
-    <t>4,16</t>
-  </si>
-  <si>
-    <t>This is the flex PCB mapping</t>
-  </si>
-  <si>
-    <t>Connecting the device to the flex PCB yields this</t>
-  </si>
-  <si>
-    <t>Flip horizontally!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">b/c we actually connect </t>
-  </si>
-  <si>
-    <t xml:space="preserve">U4 (flex pcb layout) to </t>
-  </si>
-  <si>
-    <t>U1 (rigid pcb adapter)</t>
-  </si>
-  <si>
-    <t>Showing metal pins side (metal pins visible on this side)</t>
-  </si>
-  <si>
-    <t>MAP THIS TO "KLMNO" next sheet</t>
-  </si>
-  <si>
-    <t>Orientation shown</t>
   </si>
   <si>
     <t xml:space="preserve">Orientation </t>
@@ -486,7 +497,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -553,12 +564,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -566,6 +575,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -749,8 +759,8 @@
       <xdr:rowOff>9180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>619504</xdr:colOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>379</xdr:colOff>
       <xdr:row>57</xdr:row>
       <xdr:rowOff>173845</xdr:rowOff>
     </xdr:to>
@@ -1535,19 +1545,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6C61569-4CB7-4B54-8128-A7B4B06F771A}">
-  <dimension ref="A1:R64"/>
+  <dimension ref="A1:AA64"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W32" sqref="W32"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1:Z14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A1" s="9">
+    <row r="1" spans="1:27">
+      <c r="A1" s="7">
         <v>70</v>
       </c>
-      <c r="B1" s="9">
+      <c r="B1" s="7">
         <v>71</v>
       </c>
       <c r="C1" s="1">
@@ -1569,35 +1579,60 @@
         <v>36</v>
       </c>
       <c r="K1" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L1" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="M1" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="N1" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="O1" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="P1" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="Q1" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="R1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A2" s="9">
+        <v>7</v>
+      </c>
+      <c r="T1">
+        <f t="shared" ref="T1:T13" si="0">T2-0.01</f>
+        <v>1.0099999999999998</v>
+      </c>
+      <c r="U1">
+        <v>1.19</v>
+      </c>
+      <c r="V1">
+        <v>2.0499999999999998</v>
+      </c>
+      <c r="W1">
+        <v>2.23</v>
+      </c>
+      <c r="X1">
+        <v>3.09</v>
+      </c>
+      <c r="Y1">
+        <v>3.27</v>
+      </c>
+      <c r="Z1">
+        <v>4.13</v>
+      </c>
+      <c r="AA1">
+        <v>4.3099999999999996</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27">
+      <c r="A2" s="7">
         <v>68</v>
       </c>
-      <c r="B2" s="9">
+      <c r="B2" s="7">
         <v>69</v>
       </c>
       <c r="C2" s="1">
@@ -1619,35 +1654,64 @@
         <v>38</v>
       </c>
       <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" t="s">
         <v>11</v>
       </c>
-      <c r="L2" t="s">
-        <v>19</v>
-      </c>
-      <c r="M2" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" t="s">
-        <v>21</v>
-      </c>
       <c r="O2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="P2" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="Q2" t="s">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="R2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A3" s="9">
+        <v>15</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>1.0199999999999998</v>
+      </c>
+      <c r="U2">
+        <v>1.18</v>
+      </c>
+      <c r="V2">
+        <v>2.04</v>
+      </c>
+      <c r="W2">
+        <f>W1-0.01</f>
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="X2">
+        <f>X1-0.01</f>
+        <v>3.08</v>
+      </c>
+      <c r="Y2">
+        <f>Y1-0.01</f>
+        <v>3.2600000000000002</v>
+      </c>
+      <c r="Z2">
+        <f>Z1-0.01</f>
+        <v>4.12</v>
+      </c>
+      <c r="AA2">
+        <v>4.32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27">
+      <c r="A3" s="7">
         <v>66</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="7">
         <v>67</v>
       </c>
       <c r="C3" s="1">
@@ -1669,35 +1733,64 @@
         <v>40</v>
       </c>
       <c r="K3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="M3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="N3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="O3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="P3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="Q3" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="R3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A4" s="9">
+        <v>23</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="0"/>
+        <v>1.0299999999999998</v>
+      </c>
+      <c r="U3">
+        <v>1.17</v>
+      </c>
+      <c r="V3">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W7" si="1">W2-0.01</f>
+        <v>2.2100000000000004</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X9" si="2">X2-0.01</f>
+        <v>3.0700000000000003</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y11" si="3">Y2-0.01</f>
+        <v>3.2500000000000004</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z12" si="4">Z2-0.01</f>
+        <v>4.1100000000000003</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>4.3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27">
+      <c r="A4" s="7">
         <v>64</v>
       </c>
-      <c r="B4" s="9">
+      <c r="B4" s="7">
         <v>65</v>
       </c>
       <c r="C4" s="1">
@@ -1719,35 +1812,65 @@
         <v>42</v>
       </c>
       <c r="K4" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="M4" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="O4" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="P4" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="R4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A5" s="9">
+        <v>31</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="0"/>
+        <v>1.0399999999999998</v>
+      </c>
+      <c r="U4" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="V4">
+        <v>2.02</v>
+      </c>
+      <c r="W4" s="8">
+        <f t="shared" si="1"/>
+        <v>2.2000000000000006</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="2"/>
+        <v>3.0600000000000005</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="3"/>
+        <v>3.2400000000000007</v>
+      </c>
+      <c r="Z4" s="8">
+        <f t="shared" si="4"/>
+        <v>4.1000000000000005</v>
+      </c>
+      <c r="AA4" s="8">
+        <f>AA3-0.01</f>
+        <v>4.29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27">
+      <c r="A5" s="7">
         <v>62</v>
       </c>
-      <c r="B5" s="9">
+      <c r="B5" s="7">
         <v>63</v>
       </c>
       <c r="C5" s="1">
@@ -1769,35 +1892,65 @@
         <v>44</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="M5" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="N5" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="O5" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="Q5" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="R5" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A6" s="9">
+        <v>39</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="0"/>
+        <v>1.0499999999999998</v>
+      </c>
+      <c r="U5">
+        <v>1.21</v>
+      </c>
+      <c r="V5">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="1"/>
+        <v>2.1900000000000008</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="2"/>
+        <v>3.0500000000000007</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="3"/>
+        <v>3.2300000000000009</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="4"/>
+        <v>4.0900000000000007</v>
+      </c>
+      <c r="AA5" s="8">
+        <f t="shared" ref="AA5:AA16" si="5">AA4-0.01</f>
+        <v>4.28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27">
+      <c r="A6" s="7">
         <v>60</v>
       </c>
-      <c r="B6" s="9">
+      <c r="B6" s="7">
         <v>61</v>
       </c>
       <c r="C6" s="1">
@@ -1819,31 +1972,62 @@
         <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="M6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="N6" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="O6" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="P6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="Q6" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="R6" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="0"/>
+        <v>1.0599999999999998</v>
+      </c>
+      <c r="U6">
+        <v>1.22</v>
+      </c>
+      <c r="V6">
+        <f t="shared" ref="V6:V14" si="6">V7-0.01</f>
+        <v>2.0600000000000023</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="1"/>
+        <v>2.180000000000001</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="2"/>
+        <v>3.0400000000000009</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="3"/>
+        <v>3.2200000000000011</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="4"/>
+        <v>4.080000000000001</v>
+      </c>
+      <c r="AA6" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2700000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27">
       <c r="A7" s="1">
         <v>58</v>
       </c>
@@ -1869,31 +2053,62 @@
         <v>48</v>
       </c>
       <c r="K7" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="L7" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="M7" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="N7" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="O7" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="P7" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="Q7" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="R7" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="0"/>
+        <v>1.0699999999999998</v>
+      </c>
+      <c r="U7">
+        <v>1.23</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="6"/>
+        <v>2.0700000000000021</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="1"/>
+        <v>2.1700000000000013</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="2"/>
+        <v>3.0300000000000011</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="3"/>
+        <v>3.2100000000000013</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="4"/>
+        <v>4.0700000000000012</v>
+      </c>
+      <c r="AA7" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2600000000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27">
       <c r="A8" s="1">
         <v>56</v>
       </c>
@@ -1919,31 +2134,62 @@
         <v>50</v>
       </c>
       <c r="K8" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="L8" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="M8" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="N8" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="O8" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="P8" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="Q8" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="R8" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="0"/>
+        <v>1.0799999999999998</v>
+      </c>
+      <c r="U8">
+        <v>1.24</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="6"/>
+        <v>2.0800000000000018</v>
+      </c>
+      <c r="W8" s="8">
+        <f t="shared" ref="W8:W12" si="7">W9-0.01</f>
+        <v>2.2400000000000011</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="2"/>
+        <v>3.0200000000000014</v>
+      </c>
+      <c r="Y8" s="8">
+        <f t="shared" si="3"/>
+        <v>3.2000000000000015</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="4"/>
+        <v>4.0600000000000014</v>
+      </c>
+      <c r="AA8" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2500000000000009</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27">
       <c r="A9" s="1">
         <v>54</v>
       </c>
@@ -1969,31 +2215,62 @@
         <v>52</v>
       </c>
       <c r="K9" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="N9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="O9" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="P9" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="Q9" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="R9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="0"/>
+        <v>1.0899999999999999</v>
+      </c>
+      <c r="U9">
+        <v>1.25</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="6"/>
+        <v>2.0900000000000016</v>
+      </c>
+      <c r="W9" s="8">
+        <f t="shared" si="7"/>
+        <v>2.2500000000000009</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="2"/>
+        <v>3.0100000000000016</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="3"/>
+        <v>3.1900000000000017</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="4"/>
+        <v>4.0500000000000016</v>
+      </c>
+      <c r="AA9" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2400000000000011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27">
       <c r="A10" s="1">
         <v>52</v>
       </c>
@@ -2019,31 +2296,62 @@
         <v>54</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L10" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="M10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="N10" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="O10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="P10" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="Q10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="R10" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+      <c r="T10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0999999999999999</v>
+      </c>
+      <c r="U10">
+        <v>1.26</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="6"/>
+        <v>2.1000000000000014</v>
+      </c>
+      <c r="W10" s="8">
+        <f t="shared" si="7"/>
+        <v>2.2600000000000007</v>
+      </c>
+      <c r="X10" s="8">
+        <f t="shared" ref="X10:X14" si="8">X11-0.01</f>
+        <v>3.1000000000000014</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="3"/>
+        <v>3.1800000000000019</v>
+      </c>
+      <c r="Z10">
+        <f>Z9-0.01</f>
+        <v>4.0400000000000018</v>
+      </c>
+      <c r="AA10" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2300000000000013</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27">
       <c r="A11" s="1">
         <v>50</v>
       </c>
@@ -2069,31 +2377,62 @@
         <v>56</v>
       </c>
       <c r="K11" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L11" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="M11" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="N11" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="O11" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="P11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="Q11" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="R11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="0"/>
+        <v>1.1099999999999999</v>
+      </c>
+      <c r="U11">
+        <v>1.27</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="6"/>
+        <v>2.1100000000000012</v>
+      </c>
+      <c r="W11" s="8">
+        <f t="shared" si="7"/>
+        <v>2.2700000000000005</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="8"/>
+        <v>3.1100000000000012</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="3"/>
+        <v>3.1700000000000021</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="4"/>
+        <v>4.030000000000002</v>
+      </c>
+      <c r="AA11" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2200000000000015</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27">
       <c r="A12" s="1">
         <v>48</v>
       </c>
@@ -2119,31 +2458,61 @@
         <v>58</v>
       </c>
       <c r="K12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L12" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="M12" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="N12" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="O12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="P12" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="Q12" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="R12" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="0"/>
+        <v>1.1199999999999999</v>
+      </c>
+      <c r="U12">
+        <v>1.28</v>
+      </c>
+      <c r="V12">
+        <f t="shared" si="6"/>
+        <v>2.120000000000001</v>
+      </c>
+      <c r="W12" s="8">
+        <f t="shared" si="7"/>
+        <v>2.2800000000000002</v>
+      </c>
+      <c r="X12">
+        <f t="shared" si="8"/>
+        <v>3.120000000000001</v>
+      </c>
+      <c r="Y12">
+        <v>3.28</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="4"/>
+        <v>4.0200000000000022</v>
+      </c>
+      <c r="AA12" s="8">
+        <f t="shared" si="5"/>
+        <v>4.2100000000000017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27">
       <c r="A13" s="1">
         <v>46</v>
       </c>
@@ -2169,31 +2538,61 @@
         <v>60</v>
       </c>
       <c r="K13" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L13" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="M13" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="N13" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="O13" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="P13" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="Q13" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="R13" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+      <c r="T13">
+        <f t="shared" si="0"/>
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="U13">
+        <v>1.29</v>
+      </c>
+      <c r="V13">
+        <f t="shared" si="6"/>
+        <v>2.1300000000000008</v>
+      </c>
+      <c r="W13" s="8">
+        <f>W14-0.01</f>
+        <v>2.29</v>
+      </c>
+      <c r="X13">
+        <f t="shared" si="8"/>
+        <v>3.1300000000000008</v>
+      </c>
+      <c r="Y13">
+        <v>3.29</v>
+      </c>
+      <c r="Z13">
+        <f>Z12-0.01</f>
+        <v>4.0100000000000025</v>
+      </c>
+      <c r="AA13" s="8">
+        <f t="shared" si="5"/>
+        <v>4.200000000000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27">
       <c r="A14" s="1">
         <v>44</v>
       </c>
@@ -2219,31 +2618,59 @@
         <v>62</v>
       </c>
       <c r="K14" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L14" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="M14" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="N14" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="O14" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="P14" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="Q14" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="R14" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+      <c r="T14">
+        <f>T15-0.01</f>
+        <v>1.1399999999999999</v>
+      </c>
+      <c r="U14" s="8">
+        <v>1.3</v>
+      </c>
+      <c r="V14">
+        <f t="shared" si="6"/>
+        <v>2.1400000000000006</v>
+      </c>
+      <c r="W14" s="8">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="X14">
+        <f t="shared" si="8"/>
+        <v>3.1400000000000006</v>
+      </c>
+      <c r="Y14" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="Z14">
+        <v>4.1399999999999997</v>
+      </c>
+      <c r="AA14" s="8">
+        <f t="shared" si="5"/>
+        <v>4.1900000000000022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27">
       <c r="A15" s="1">
         <v>42</v>
       </c>
@@ -2269,31 +2696,58 @@
         <v>64</v>
       </c>
       <c r="K15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="L15" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="M15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="N15" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="O15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="P15" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="Q15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="R15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+      <c r="T15">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="U15">
+        <v>1.32</v>
+      </c>
+      <c r="V15">
+        <f>V16-0.01</f>
+        <v>2.1500000000000004</v>
+      </c>
+      <c r="W15">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="X15">
+        <f>X16-0.01</f>
+        <v>3.1500000000000004</v>
+      </c>
+      <c r="Y15">
+        <v>3.32</v>
+      </c>
+      <c r="Z15">
+        <v>4.1500000000000004</v>
+      </c>
+      <c r="AA15" s="8">
+        <f t="shared" si="5"/>
+        <v>4.1800000000000024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27">
       <c r="A16" s="1">
         <v>40</v>
       </c>
@@ -2319,122 +2773,136 @@
         <v>67</v>
       </c>
       <c r="K16" t="s">
+        <v>120</v>
+      </c>
+      <c r="L16" t="s">
+        <v>121</v>
+      </c>
+      <c r="M16" t="s">
+        <v>122</v>
+      </c>
+      <c r="N16" t="s">
+        <v>123</v>
+      </c>
+      <c r="O16" t="s">
+        <v>124</v>
+      </c>
+      <c r="P16" t="s">
+        <v>125</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>126</v>
+      </c>
+      <c r="R16" t="s">
+        <v>127</v>
+      </c>
+      <c r="T16">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="U16">
+        <v>1.31</v>
+      </c>
+      <c r="V16">
+        <v>2.16</v>
+      </c>
+      <c r="W16">
+        <v>2.31</v>
+      </c>
+      <c r="X16">
+        <v>3.16</v>
+      </c>
+      <c r="Y16">
+        <v>3.31</v>
+      </c>
+      <c r="Z16">
+        <v>4.16</v>
+      </c>
+      <c r="AA16" s="8">
+        <f t="shared" si="5"/>
+        <v>4.1700000000000026</v>
+      </c>
+    </row>
+    <row r="17" spans="1:23">
+      <c r="A17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="18" spans="1:23">
+      <c r="A18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="W18" t="s">
         <v>129</v>
       </c>
-      <c r="L16" t="s">
+    </row>
+    <row r="19" spans="1:23">
+      <c r="B19" t="s">
         <v>130</v>
       </c>
-      <c r="M16" t="s">
+      <c r="G19" t="s">
         <v>131</v>
       </c>
-      <c r="N16" t="s">
+    </row>
+    <row r="21" spans="1:23">
+      <c r="B21" t="s">
         <v>132</v>
       </c>
-      <c r="O16" t="s">
+      <c r="F21" t="s">
         <v>133</v>
       </c>
-      <c r="P16" t="s">
+      <c r="W21" t="s">
         <v>134</v>
       </c>
-      <c r="Q16" t="s">
+    </row>
+    <row r="22" spans="1:23">
+      <c r="W22" t="s">
         <v>135</v>
       </c>
-      <c r="R16" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H19" s="3"/>
-    </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-    </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A21" s="3"/>
-      <c r="B21" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A23" s="9">
+    </row>
+    <row r="23" spans="1:23">
+      <c r="A23" s="7">
         <v>71</v>
       </c>
       <c r="B23" s="1">
@@ -2447,20 +2915,20 @@
         <v>36</v>
       </c>
       <c r="K23" t="s">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="L23" t="s">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="Q23" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="R23" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A24" s="9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23">
+      <c r="A24" s="7">
         <v>70</v>
       </c>
       <c r="B24" s="1">
@@ -2473,20 +2941,20 @@
         <v>37</v>
       </c>
       <c r="K24" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="L24" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="Q24" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="R24" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A25" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23">
+      <c r="A25" s="7">
         <v>69</v>
       </c>
       <c r="B25" s="1">
@@ -2499,20 +2967,20 @@
         <v>38</v>
       </c>
       <c r="K25" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="L25" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="Q25" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="R25" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A26" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23">
+      <c r="A26" s="7">
         <v>68</v>
       </c>
       <c r="B26" s="1">
@@ -2525,20 +2993,20 @@
         <v>39</v>
       </c>
       <c r="K26" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="L26" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="Q26" t="s">
-        <v>23</v>
+        <v>13</v>
       </c>
       <c r="R26" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A27" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23">
+      <c r="A27" s="7">
         <v>67</v>
       </c>
       <c r="B27" s="1">
@@ -2551,20 +3019,20 @@
         <v>40</v>
       </c>
       <c r="K27" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="L27" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="Q27" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="R27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A28" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23">
+      <c r="A28" s="7">
         <v>66</v>
       </c>
       <c r="B28" s="1">
@@ -2577,20 +3045,20 @@
         <v>41</v>
       </c>
       <c r="K28" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L28" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="Q28" t="s">
+        <v>21</v>
+      </c>
+      <c r="R28" t="s">
         <v>30</v>
       </c>
-      <c r="R28" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A29" s="9">
+    </row>
+    <row r="29" spans="1:23">
+      <c r="A29" s="7">
         <v>65</v>
       </c>
       <c r="B29" s="1">
@@ -2603,20 +3071,20 @@
         <v>42</v>
       </c>
       <c r="K29" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="L29" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="Q29" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="R29" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A30" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23">
+      <c r="A30" s="7">
         <v>64</v>
       </c>
       <c r="B30" s="1">
@@ -2629,20 +3097,20 @@
         <v>43</v>
       </c>
       <c r="K30" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="L30" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="Q30" t="s">
+        <v>29</v>
+      </c>
+      <c r="R30" t="s">
         <v>38</v>
       </c>
-      <c r="R30" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A31" s="9">
+    </row>
+    <row r="31" spans="1:23">
+      <c r="A31" s="7">
         <v>63</v>
       </c>
       <c r="B31" s="1">
@@ -2655,27 +3123,27 @@
         <v>44</v>
       </c>
       <c r="K31" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="L31" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="Q31" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="R31" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A32" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:23">
+      <c r="A32" s="7">
         <v>62</v>
       </c>
       <c r="B32" s="1">
         <v>26</v>
       </c>
       <c r="D32" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G32" s="2">
         <v>10</v>
@@ -2684,20 +3152,20 @@
         <v>45</v>
       </c>
       <c r="K32" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="L32" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="Q32" t="s">
+        <v>37</v>
+      </c>
+      <c r="R32" t="s">
         <v>46</v>
       </c>
-      <c r="R32" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A33" s="9">
+    </row>
+    <row r="33" spans="1:18">
+      <c r="A33" s="7">
         <v>61</v>
       </c>
       <c r="B33" s="1">
@@ -2710,19 +3178,19 @@
         <v>46</v>
       </c>
       <c r="K33" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="L33" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="Q33" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="R33" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" x14ac:dyDescent="0.4">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18">
       <c r="A34" s="1">
         <v>60</v>
       </c>
@@ -2736,19 +3204,19 @@
         <v>47</v>
       </c>
       <c r="K34" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="L34" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="Q34" t="s">
+        <v>45</v>
+      </c>
+      <c r="R34" t="s">
         <v>54</v>
       </c>
-      <c r="R34" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="35" spans="1:18">
       <c r="A35" s="1">
         <v>59</v>
       </c>
@@ -2762,19 +3230,19 @@
         <v>48</v>
       </c>
       <c r="K35" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="L35" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="Q35" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="R35" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.4">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18">
       <c r="A36" s="1">
         <v>58</v>
       </c>
@@ -2788,19 +3256,19 @@
         <v>49</v>
       </c>
       <c r="K36" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="L36" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="Q36" t="s">
+        <v>53</v>
+      </c>
+      <c r="R36" t="s">
         <v>62</v>
       </c>
-      <c r="R36" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="37" spans="1:18">
       <c r="A37" s="1">
         <v>57</v>
       </c>
@@ -2814,19 +3282,19 @@
         <v>50</v>
       </c>
       <c r="K37" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="L37" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="Q37" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="R37" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.4">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18">
       <c r="A38" s="1">
         <v>56</v>
       </c>
@@ -2840,19 +3308,19 @@
         <v>51</v>
       </c>
       <c r="K38" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="L38" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="Q38" t="s">
+        <v>61</v>
+      </c>
+      <c r="R38" t="s">
         <v>70</v>
       </c>
-      <c r="R38" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="39" spans="1:18">
       <c r="A39" s="1">
         <v>55</v>
       </c>
@@ -2866,19 +3334,19 @@
         <v>52</v>
       </c>
       <c r="K39" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="L39" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="Q39" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="R39" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.4">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18">
       <c r="A40" s="1">
         <v>54</v>
       </c>
@@ -2892,19 +3360,19 @@
         <v>53</v>
       </c>
       <c r="K40" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="L40" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="Q40" t="s">
+        <v>69</v>
+      </c>
+      <c r="R40" t="s">
         <v>78</v>
       </c>
-      <c r="R40" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="41" spans="1:18">
       <c r="A41" s="1">
         <v>53</v>
       </c>
@@ -2918,19 +3386,19 @@
         <v>54</v>
       </c>
       <c r="K41" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="L41" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="Q41" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="R41" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.4">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="42" spans="1:18">
       <c r="A42" s="1">
         <v>52</v>
       </c>
@@ -2944,19 +3412,19 @@
         <v>55</v>
       </c>
       <c r="K42" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="L42" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="Q42" t="s">
+        <v>77</v>
+      </c>
+      <c r="R42" t="s">
         <v>86</v>
       </c>
-      <c r="R42" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="43" spans="1:18">
       <c r="A43" s="1">
         <v>51</v>
       </c>
@@ -2970,19 +3438,19 @@
         <v>56</v>
       </c>
       <c r="K43" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="L43" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="Q43" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="R43" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.4">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18">
       <c r="A44" s="1">
         <v>50</v>
       </c>
@@ -2996,19 +3464,19 @@
         <v>57</v>
       </c>
       <c r="K44" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="L44" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="Q44" t="s">
+        <v>85</v>
+      </c>
+      <c r="R44" t="s">
         <v>94</v>
       </c>
-      <c r="R44" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="45" spans="1:18">
       <c r="A45" s="1">
         <v>49</v>
       </c>
@@ -3022,19 +3490,19 @@
         <v>58</v>
       </c>
       <c r="K45" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="L45" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="Q45" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="R45" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.4">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:18">
       <c r="A46" s="1">
         <v>48</v>
       </c>
@@ -3048,19 +3516,19 @@
         <v>59</v>
       </c>
       <c r="K46" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="L46" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="Q46" t="s">
+        <v>93</v>
+      </c>
+      <c r="R46" t="s">
         <v>102</v>
       </c>
-      <c r="R46" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="47" spans="1:18">
       <c r="A47" s="1">
         <v>47</v>
       </c>
@@ -3074,19 +3542,19 @@
         <v>60</v>
       </c>
       <c r="K47" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="L47" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="Q47" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="R47" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.4">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3100,19 +3568,19 @@
         <v>61</v>
       </c>
       <c r="K48" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="L48" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="Q48" t="s">
+        <v>101</v>
+      </c>
+      <c r="R48" t="s">
         <v>110</v>
       </c>
-      <c r="R48" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="49" spans="1:18">
       <c r="A49" s="1">
         <v>45</v>
       </c>
@@ -3126,19 +3594,19 @@
         <v>62</v>
       </c>
       <c r="K49" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="L49" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="Q49" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="R49" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.4">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18">
       <c r="A50" s="1">
         <v>44</v>
       </c>
@@ -3152,19 +3620,19 @@
         <v>63</v>
       </c>
       <c r="K50" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="L50" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="Q50" t="s">
+        <v>109</v>
+      </c>
+      <c r="R50" t="s">
         <v>118</v>
       </c>
-      <c r="R50" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="51" spans="1:18" x14ac:dyDescent="0.4">
+    </row>
+    <row r="51" spans="1:18">
       <c r="A51" s="1">
         <v>43</v>
       </c>
@@ -3178,19 +3646,19 @@
         <v>64</v>
       </c>
       <c r="K51" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="L51" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="Q51" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="R51" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" x14ac:dyDescent="0.4">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18">
       <c r="A52" s="1">
         <v>42</v>
       </c>
@@ -3204,19 +3672,19 @@
         <v>65</v>
       </c>
       <c r="K52" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="L52" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="Q52" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="R52" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="53" spans="1:18" x14ac:dyDescent="0.4">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18">
       <c r="A53" s="1">
         <v>41</v>
       </c>
@@ -3230,19 +3698,19 @@
         <v>66</v>
       </c>
       <c r="K53" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="L53" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="Q53" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="R53" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" x14ac:dyDescent="0.4">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18">
       <c r="A54" s="1">
         <v>40</v>
       </c>
@@ -3256,90 +3724,90 @@
         <v>67</v>
       </c>
       <c r="K54" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="L54" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="Q54" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="R54" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A55" s="6">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18">
+      <c r="A55" s="4">
         <v>39</v>
       </c>
-      <c r="B55" s="6">
+      <c r="B55" s="4">
         <v>3</v>
       </c>
-      <c r="G55" s="6">
+      <c r="G55" s="4">
         <v>33</v>
       </c>
-      <c r="H55" s="6">
+      <c r="H55" s="4">
         <v>68</v>
       </c>
     </row>
-    <row r="56" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A56" s="6">
+    <row r="56" spans="1:18">
+      <c r="A56" s="4">
         <v>38</v>
       </c>
-      <c r="B56" s="6">
+      <c r="B56" s="4">
         <v>2</v>
       </c>
       <c r="C56" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="F56" t="s">
-        <v>6</v>
-      </c>
-      <c r="G56" s="6">
+        <v>138</v>
+      </c>
+      <c r="G56" s="4">
         <v>34</v>
       </c>
-      <c r="H56" s="6">
+      <c r="H56" s="4">
         <v>69</v>
       </c>
     </row>
-    <row r="57" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A57" s="6">
+    <row r="57" spans="1:18">
+      <c r="A57" s="4">
         <v>37</v>
       </c>
-      <c r="B57" s="6">
+      <c r="B57" s="4">
         <v>1</v>
       </c>
-      <c r="G57" s="6">
+      <c r="G57" s="4">
         <v>35</v>
       </c>
-      <c r="H57" s="6">
+      <c r="H57" s="4">
         <v>70</v>
       </c>
     </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.4">
-      <c r="A58" s="6">
+    <row r="58" spans="1:18">
+      <c r="A58" s="4">
         <v>36</v>
       </c>
-      <c r="B58" s="6"/>
-      <c r="G58" s="6"/>
-      <c r="H58" s="6">
+      <c r="B58" s="4"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4">
         <v>71</v>
       </c>
     </row>
-    <row r="62" spans="1:18" ht="38.6" x14ac:dyDescent="1">
-      <c r="A62" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="K62" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:18" ht="38.65">
+      <c r="A62" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="K62" s="6" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18">
       <c r="C64" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="M64" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
   </sheetData>
@@ -3355,29 +3823,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20421E89-A308-41F9-B187-726133438ABA}">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="97" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:15">
       <c r="A1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5"/>
+        <v>130</v>
+      </c>
+      <c r="B1" s="3"/>
       <c r="D1" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="L1" t="s">
-        <v>3</v>
-      </c>
-      <c r="N1" s="5"/>
+        <v>131</v>
+      </c>
+      <c r="N1" s="3"/>
       <c r="O1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.4">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2">
         <v>63</v>
       </c>
@@ -3403,7 +3871,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:15">
       <c r="A3">
         <v>62</v>
       </c>
@@ -3429,7 +3897,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:15">
       <c r="A4">
         <v>61</v>
       </c>
@@ -3455,7 +3923,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:15">
       <c r="A5">
         <v>60</v>
       </c>
@@ -3481,7 +3949,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:15">
       <c r="A6">
         <v>59</v>
       </c>
@@ -3507,7 +3975,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:15">
       <c r="A7">
         <v>58</v>
       </c>
@@ -3533,7 +4001,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:15">
       <c r="A8">
         <v>57</v>
       </c>
@@ -3559,7 +4027,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:15">
       <c r="A9">
         <v>56</v>
       </c>
@@ -3585,7 +4053,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:15">
       <c r="A10">
         <v>55</v>
       </c>
@@ -3611,7 +4079,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:15">
       <c r="A11">
         <v>54</v>
       </c>
@@ -3637,7 +4105,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:15">
       <c r="A12">
         <v>53</v>
       </c>
@@ -3663,7 +4131,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:15">
       <c r="A13">
         <v>52</v>
       </c>
@@ -3689,7 +4157,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:15">
       <c r="A14">
         <v>51</v>
       </c>
@@ -3715,7 +4183,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:15">
       <c r="A15">
         <v>50</v>
       </c>
@@ -3729,7 +4197,7 @@
         <v>77</v>
       </c>
       <c r="H15" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
       <c r="K15">
         <v>77</v>
@@ -3744,7 +4212,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:15">
       <c r="A16">
         <v>49</v>
       </c>
@@ -3758,7 +4226,7 @@
         <v>78</v>
       </c>
       <c r="H16" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
       <c r="K16">
         <v>78</v>
@@ -3773,7 +4241,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:15">
       <c r="A17">
         <v>48</v>
       </c>
@@ -3799,7 +4267,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:15">
       <c r="A18">
         <v>47</v>
       </c>
@@ -3813,7 +4281,7 @@
         <v>80</v>
       </c>
       <c r="H18" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
       <c r="K18">
         <v>80</v>
@@ -3828,7 +4296,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:15">
       <c r="A19">
         <v>46</v>
       </c>
@@ -3842,7 +4310,7 @@
         <v>81</v>
       </c>
       <c r="H19" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
       <c r="K19">
         <v>81</v>
@@ -3857,7 +4325,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:15">
       <c r="A20">
         <v>45</v>
       </c>
@@ -3883,7 +4351,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:15">
       <c r="A21">
         <v>44</v>
       </c>
@@ -3909,7 +4377,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:15">
       <c r="A22">
         <v>43</v>
       </c>
@@ -3935,7 +4403,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:15">
       <c r="A23">
         <v>42</v>
       </c>
@@ -3961,7 +4429,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:15">
       <c r="A24">
         <v>41</v>
       </c>
@@ -3987,7 +4455,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:15">
       <c r="A25">
         <v>40</v>
       </c>
@@ -4013,7 +4481,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:15">
       <c r="A26">
         <v>39</v>
       </c>
@@ -4039,7 +4507,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:15">
       <c r="A27">
         <v>38</v>
       </c>
@@ -4065,7 +4533,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:15">
       <c r="A28">
         <v>37</v>
       </c>
@@ -4091,7 +4559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:15">
       <c r="A29">
         <v>36</v>
       </c>
@@ -4117,7 +4585,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:15">
       <c r="A30">
         <v>35</v>
       </c>
@@ -4143,7 +4611,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:15">
       <c r="A31">
         <v>34</v>
       </c>
@@ -4169,7 +4637,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:15">
       <c r="A32">
         <v>33</v>
       </c>
@@ -4195,7 +4663,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:15">
       <c r="A33">
         <v>32</v>
       </c>
@@ -4221,135 +4689,135 @@
         <v>32</v>
       </c>
     </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N34" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O34" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O35" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E36" s="5" t="s">
-        <v>5</v>
+    <row r="34" spans="1:15">
+      <c r="A34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N34" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O34" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15">
+      <c r="A35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N35" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O35" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15">
+      <c r="A36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>147</v>
       </c>
       <c r="G36" t="s">
-        <v>8</v>
-      </c>
-      <c r="K36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N36" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O36" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.4">
-      <c r="A37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="K37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="L37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="N37" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O37" s="5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.4">
+        <v>148</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N36" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O36" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15">
+      <c r="A37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="L37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="N37" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="O37" s="3" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15">
       <c r="A40" t="s">
-        <v>7</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="L40" t="s">
-        <v>6</v>
+        <v>138</v>
       </c>
       <c r="O40" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.4">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15">
       <c r="E43" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.4">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15">
       <c r="E44" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
@@ -4369,9 +4837,9 @@
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="14.65"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4">
       <c r="A1">
         <v>67</v>
       </c>
@@ -4385,7 +4853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>65</v>
       </c>
@@ -4399,7 +4867,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>69</v>
       </c>
@@ -4413,7 +4881,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>71</v>
       </c>
@@ -4427,7 +4895,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>73</v>
       </c>
@@ -4441,7 +4909,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>75</v>
       </c>
@@ -4455,7 +4923,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>77</v>
       </c>
@@ -4469,7 +4937,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>79</v>
       </c>
@@ -4483,7 +4951,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:4">
       <c r="A9">
         <v>81</v>
       </c>
@@ -4497,7 +4965,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:4">
       <c r="A10">
         <v>83</v>
       </c>
@@ -4511,7 +4979,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>85</v>
       </c>
@@ -4525,7 +4993,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>87</v>
       </c>
@@ -4539,7 +5007,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>89</v>
       </c>
@@ -4553,7 +5021,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>91</v>
       </c>
@@ -4567,7 +5035,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>93</v>
       </c>
@@ -4581,7 +5049,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>95</v>
       </c>
@@ -4595,7 +5063,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:4">
       <c r="A17">
         <v>94</v>
       </c>
@@ -4609,7 +5077,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:4">
       <c r="A18">
         <v>92</v>
       </c>
@@ -4623,7 +5091,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:4">
       <c r="A19">
         <v>90</v>
       </c>
@@ -4637,7 +5105,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:4">
       <c r="A20">
         <v>64</v>
       </c>
@@ -4651,7 +5119,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:4">
       <c r="A21">
         <v>66</v>
       </c>
@@ -4665,7 +5133,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:4">
       <c r="A22">
         <v>68</v>
       </c>
@@ -4679,7 +5147,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:4">
       <c r="A23">
         <v>70</v>
       </c>
@@ -4693,7 +5161,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:4">
       <c r="A24">
         <v>72</v>
       </c>
@@ -4707,7 +5175,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:4">
       <c r="A25">
         <v>74</v>
       </c>
@@ -4721,7 +5189,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:4">
       <c r="A26">
         <v>76</v>
       </c>
@@ -4735,7 +5203,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:4">
       <c r="A27">
         <v>78</v>
       </c>
@@ -4749,7 +5217,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:4">
       <c r="A28">
         <v>80</v>
       </c>
@@ -4763,7 +5231,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:4">
       <c r="A29">
         <v>82</v>
       </c>
@@ -4777,7 +5245,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:4">
       <c r="A30">
         <v>84</v>
       </c>
@@ -4791,7 +5259,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:4">
       <c r="A31">
         <v>86</v>
       </c>
@@ -4805,7 +5273,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:4">
       <c r="A32">
         <v>88</v>
       </c>

</xml_diff>